<commit_message>
fixed to use localhosted docker
</commit_message>
<xml_diff>
--- a/sampledata.xlsx
+++ b/sampledata.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\GitHub\PetTestCharlie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F0E68F6-78A4-4407-BA89-2B1D1BAF238F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{311E990F-53F7-4C7C-BA09-80F619FE6D6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="46035" yWindow="3135" windowWidth="21180" windowHeight="15285" xr2:uid="{F2BF25C8-0339-43A8-BA0D-D8B697DB61F0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{E5E42642-9A87-4870-8963-9DF0E67F62F7}"/>
   </bookViews>
   <sheets>
-    <sheet name="sampledata" sheetId="1" r:id="rId1"/>
+    <sheet name="data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="187">
   <si>
     <t>Pet</t>
   </si>
@@ -37,21 +37,342 @@
     <t>Canine</t>
   </si>
   <si>
+    <t>2024-10-06 16:44</t>
+  </si>
+  <si>
+    <t>270</t>
+  </si>
+  <si>
+    <t>mg/dL</t>
+  </si>
+  <si>
+    <t>2024-10-06 14:49</t>
+  </si>
+  <si>
+    <t>150</t>
+  </si>
+  <si>
+    <t>2024-10-06 10:56</t>
+  </si>
+  <si>
+    <t>93</t>
+  </si>
+  <si>
+    <t>2024-10-06 06:14</t>
+  </si>
+  <si>
+    <t>2024-10-05 19:01</t>
+  </si>
+  <si>
+    <t>111</t>
+  </si>
+  <si>
+    <t>2024-10-05 14:30</t>
+  </si>
+  <si>
+    <t>146</t>
+  </si>
+  <si>
+    <t>2024-10-05 10:22</t>
+  </si>
+  <si>
+    <t>265</t>
+  </si>
+  <si>
+    <t>2024-10-05 06:29</t>
+  </si>
+  <si>
+    <t>49</t>
+  </si>
+  <si>
+    <t>2024-10-04 18:10</t>
+  </si>
+  <si>
+    <t>497</t>
+  </si>
+  <si>
+    <t>2024-10-04 15:22</t>
+  </si>
+  <si>
+    <t>214</t>
+  </si>
+  <si>
+    <t>2024-10-04 11:31</t>
+  </si>
+  <si>
+    <t>216</t>
+  </si>
+  <si>
+    <t>2024-10-04 06:35</t>
+  </si>
+  <si>
+    <t>282</t>
+  </si>
+  <si>
+    <t>2024-10-03 18:08</t>
+  </si>
+  <si>
+    <t>414</t>
+  </si>
+  <si>
+    <t>2024-10-03 15:42</t>
+  </si>
+  <si>
+    <t>280</t>
+  </si>
+  <si>
+    <t>2024-10-03 10:38</t>
+  </si>
+  <si>
+    <t>180</t>
+  </si>
+  <si>
+    <t>2024-10-03 06:10</t>
+  </si>
+  <si>
+    <t>88</t>
+  </si>
+  <si>
+    <t>2024-10-02 14:53</t>
+  </si>
+  <si>
+    <t>243</t>
+  </si>
+  <si>
+    <t>2024-10-02 11:29</t>
+  </si>
+  <si>
+    <t>299</t>
+  </si>
+  <si>
+    <t>2024-10-02 06:42</t>
+  </si>
+  <si>
+    <t>160</t>
+  </si>
+  <si>
+    <t>2024-10-01 18:17</t>
+  </si>
+  <si>
+    <t>419</t>
+  </si>
+  <si>
+    <t>2024-10-01 14:45</t>
+  </si>
+  <si>
+    <t>245</t>
+  </si>
+  <si>
+    <t>2024-10-01 10:34</t>
+  </si>
+  <si>
+    <t>305</t>
+  </si>
+  <si>
+    <t>2024-10-01 06:49</t>
+  </si>
+  <si>
+    <t>79</t>
+  </si>
+  <si>
+    <t>2024-09-30 18:38</t>
+  </si>
+  <si>
+    <t>417</t>
+  </si>
+  <si>
+    <t>2024-09-30 15:43</t>
+  </si>
+  <si>
+    <t>352</t>
+  </si>
+  <si>
+    <t>2024-09-30 11:59</t>
+  </si>
+  <si>
+    <t>2024-09-30 06:38</t>
+  </si>
+  <si>
+    <t>149</t>
+  </si>
+  <si>
+    <t>2024-09-29 18:09</t>
+  </si>
+  <si>
+    <t>209</t>
+  </si>
+  <si>
+    <t>2024-09-29 14:44</t>
+  </si>
+  <si>
+    <t>367</t>
+  </si>
+  <si>
+    <t>2024-09-29 11:57</t>
+  </si>
+  <si>
+    <t>77</t>
+  </si>
+  <si>
+    <t>2024-09-29 06:01</t>
+  </si>
+  <si>
+    <t>126</t>
+  </si>
+  <si>
+    <t>2024-09-28 18:07</t>
+  </si>
+  <si>
+    <t>152</t>
+  </si>
+  <si>
+    <t>2024-09-27 18:59</t>
+  </si>
+  <si>
+    <t>259</t>
+  </si>
+  <si>
+    <t>2024-09-27 14:26</t>
+  </si>
+  <si>
+    <t>177</t>
+  </si>
+  <si>
+    <t>2024-09-27 10:54</t>
+  </si>
+  <si>
+    <t>104</t>
+  </si>
+  <si>
+    <t>2024-09-27 06:26</t>
+  </si>
+  <si>
+    <t>80</t>
+  </si>
+  <si>
+    <t>2024-09-26 18:19</t>
+  </si>
+  <si>
+    <t>524</t>
+  </si>
+  <si>
+    <t>2024-09-26 15:39</t>
+  </si>
+  <si>
+    <t>221</t>
+  </si>
+  <si>
+    <t>2024-09-26 11:10</t>
+  </si>
+  <si>
+    <t>2024-09-26 05:26</t>
+  </si>
+  <si>
+    <t>108</t>
+  </si>
+  <si>
+    <t>2024-09-25 18:14</t>
+  </si>
+  <si>
+    <t>385</t>
+  </si>
+  <si>
+    <t>2024-09-25 16:03</t>
+  </si>
+  <si>
+    <t>457</t>
+  </si>
+  <si>
+    <t>2024-09-25 14:27</t>
+  </si>
+  <si>
+    <t>237</t>
+  </si>
+  <si>
+    <t>2024-09-25 10:13</t>
+  </si>
+  <si>
+    <t>202</t>
+  </si>
+  <si>
+    <t>2024-09-25 06:53</t>
+  </si>
+  <si>
+    <t>94</t>
+  </si>
+  <si>
+    <t>2024-09-24 18:25</t>
+  </si>
+  <si>
+    <t>500</t>
+  </si>
+  <si>
+    <t>2024-09-24 16:02</t>
+  </si>
+  <si>
+    <t>2024-09-24 12:29</t>
+  </si>
+  <si>
+    <t>82</t>
+  </si>
+  <si>
+    <t>2024-09-24 06:35</t>
+  </si>
+  <si>
+    <t>76</t>
+  </si>
+  <si>
+    <t>2024-09-23 22:35</t>
+  </si>
+  <si>
+    <t>157</t>
+  </si>
+  <si>
+    <t>2024-09-23 18:11</t>
+  </si>
+  <si>
+    <t>514</t>
+  </si>
+  <si>
+    <t>2024-09-23 15:55</t>
+  </si>
+  <si>
+    <t>275</t>
+  </si>
+  <si>
+    <t>2024-09-23 11:50</t>
+  </si>
+  <si>
+    <t>205</t>
+  </si>
+  <si>
+    <t>2024-09-23 06:41</t>
+  </si>
+  <si>
+    <t>145</t>
+  </si>
+  <si>
+    <t>2024-09-22 20:52</t>
+  </si>
+  <si>
+    <t>428</t>
+  </si>
+  <si>
+    <t>2024-09-22 16:05</t>
+  </si>
+  <si>
+    <t>57</t>
+  </si>
+  <si>
     <t>2024-09-22 12:57</t>
   </si>
   <si>
     <t>54</t>
   </si>
   <si>
-    <t>mg/dL</t>
-  </si>
-  <si>
     <t>2024-09-22 06:48</t>
   </si>
   <si>
-    <t>77</t>
-  </si>
-  <si>
     <t>2024-09-21 19:52</t>
   </si>
   <si>
@@ -94,9 +415,6 @@
     <t>2024-09-20 09:13</t>
   </si>
   <si>
-    <t>497</t>
-  </si>
-  <si>
     <t>2024-09-20 03:54</t>
   </si>
   <si>
@@ -130,9 +448,6 @@
     <t>2024-09-18 18:38</t>
   </si>
   <si>
-    <t>417</t>
-  </si>
-  <si>
     <t>2024-09-18 15:48</t>
   </si>
   <si>
@@ -187,9 +502,6 @@
     <t>2024-09-15 16:00</t>
   </si>
   <si>
-    <t>202</t>
-  </si>
-  <si>
     <t>2024-09-15 06:20</t>
   </si>
   <si>
@@ -263,9 +575,6 @@
   </si>
   <si>
     <t>2024-09-11 12:06</t>
-  </si>
-  <si>
-    <t>275</t>
   </si>
   <si>
     <t>2024-09-11 05:53</t>
@@ -278,6 +587,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.0"/>
+  </numFmts>
   <fonts count="1">
     <font>
       <sz val="12"/>
@@ -304,9 +616,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
@@ -643,23 +964,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69254C3D-5C1B-4BBA-8FC8-4851047FCF18}">
-  <dimension ref="A3:D46"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2F74B97-00E6-4BF5-9F8F-3459C71C3F01}">
+  <dimension ref="A3:D99"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:C99"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="2" width="18.453125" customWidth="1"/>
-    <col min="3" max="11" width="12" customWidth="1"/>
+    <col min="2" max="2" width="15.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="12" width="12" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -673,10 +996,10 @@
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -687,10 +1010,10 @@
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -701,10 +1024,10 @@
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -715,11 +1038,11 @@
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>13</v>
+      <c r="C7" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>7</v>
@@ -729,11 +1052,11 @@
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>14</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>7</v>
@@ -743,11 +1066,11 @@
       <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>7</v>
@@ -757,11 +1080,11 @@
       <c r="A10" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>18</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>7</v>
@@ -771,11 +1094,11 @@
       <c r="A11" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>20</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>7</v>
@@ -785,11 +1108,11 @@
       <c r="A12" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>7</v>
@@ -799,10 +1122,10 @@
       <c r="A13" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="4" t="s">
         <v>24</v>
       </c>
       <c r="D13" s="1" t="s">
@@ -813,10 +1136,10 @@
       <c r="A14" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="4" t="s">
         <v>26</v>
       </c>
       <c r="D14" s="1" t="s">
@@ -827,10 +1150,10 @@
       <c r="A15" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="4" t="s">
         <v>28</v>
       </c>
       <c r="D15" s="1" t="s">
@@ -841,10 +1164,10 @@
       <c r="A16" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D16" s="1" t="s">
@@ -855,10 +1178,10 @@
       <c r="A17" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="4" t="s">
         <v>32</v>
       </c>
       <c r="D17" s="1" t="s">
@@ -869,10 +1192,10 @@
       <c r="A18" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="4" t="s">
         <v>34</v>
       </c>
       <c r="D18" s="1" t="s">
@@ -883,10 +1206,10 @@
       <c r="A19" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="4" t="s">
         <v>36</v>
       </c>
       <c r="D19" s="1" t="s">
@@ -897,10 +1220,10 @@
       <c r="A20" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" s="4" t="s">
         <v>38</v>
       </c>
       <c r="D20" s="1" t="s">
@@ -911,10 +1234,10 @@
       <c r="A21" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" s="4" t="s">
         <v>40</v>
       </c>
       <c r="D21" s="1" t="s">
@@ -925,10 +1248,10 @@
       <c r="A22" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" s="4" t="s">
         <v>42</v>
       </c>
       <c r="D22" s="1" t="s">
@@ -939,10 +1262,10 @@
       <c r="A23" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" s="4" t="s">
         <v>44</v>
       </c>
       <c r="D23" s="1" t="s">
@@ -953,10 +1276,10 @@
       <c r="A24" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" s="4" t="s">
         <v>46</v>
       </c>
       <c r="D24" s="1" t="s">
@@ -967,10 +1290,10 @@
       <c r="A25" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" s="4" t="s">
         <v>48</v>
       </c>
       <c r="D25" s="1" t="s">
@@ -981,10 +1304,10 @@
       <c r="A26" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" s="4" t="s">
         <v>50</v>
       </c>
       <c r="D26" s="1" t="s">
@@ -995,10 +1318,10 @@
       <c r="A27" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C27" s="4" t="s">
         <v>52</v>
       </c>
       <c r="D27" s="1" t="s">
@@ -1009,11 +1332,11 @@
       <c r="A28" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>9</v>
+      <c r="C28" s="4" t="s">
+        <v>54</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>7</v>
@@ -1023,11 +1346,11 @@
       <c r="A29" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C29" s="1" t="s">
+      <c r="B29" s="2" t="s">
         <v>55</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>7</v>
@@ -1037,10 +1360,10 @@
       <c r="A30" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C30" s="4" t="s">
         <v>57</v>
       </c>
       <c r="D30" s="1" t="s">
@@ -1051,10 +1374,10 @@
       <c r="A31" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C31" s="4" t="s">
         <v>59</v>
       </c>
       <c r="D31" s="1" t="s">
@@ -1065,10 +1388,10 @@
       <c r="A32" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C32" s="4" t="s">
         <v>61</v>
       </c>
       <c r="D32" s="1" t="s">
@@ -1079,10 +1402,10 @@
       <c r="A33" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B33" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C33" s="4" t="s">
         <v>63</v>
       </c>
       <c r="D33" s="1" t="s">
@@ -1093,10 +1416,10 @@
       <c r="A34" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B34" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C34" s="4" t="s">
         <v>65</v>
       </c>
       <c r="D34" s="1" t="s">
@@ -1107,10 +1430,10 @@
       <c r="A35" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B35" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C35" s="4" t="s">
         <v>67</v>
       </c>
       <c r="D35" s="1" t="s">
@@ -1121,10 +1444,10 @@
       <c r="A36" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B36" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C36" s="4" t="s">
         <v>69</v>
       </c>
       <c r="D36" s="1" t="s">
@@ -1135,10 +1458,10 @@
       <c r="A37" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B37" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C37" s="4" t="s">
         <v>71</v>
       </c>
       <c r="D37" s="1" t="s">
@@ -1149,10 +1472,10 @@
       <c r="A38" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B38" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="C38" s="4" t="s">
         <v>73</v>
       </c>
       <c r="D38" s="1" t="s">
@@ -1163,10 +1486,10 @@
       <c r="A39" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B39" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C39" s="4" t="s">
         <v>75</v>
       </c>
       <c r="D39" s="1" t="s">
@@ -1177,10 +1500,10 @@
       <c r="A40" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B40" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C40" s="4" t="s">
         <v>77</v>
       </c>
       <c r="D40" s="1" t="s">
@@ -1191,10 +1514,10 @@
       <c r="A41" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B41" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C41" s="4" t="s">
         <v>79</v>
       </c>
       <c r="D41" s="1" t="s">
@@ -1205,11 +1528,11 @@
       <c r="A42" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B42" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C42" s="1" t="s">
-        <v>81</v>
+      <c r="C42" s="4" t="s">
+        <v>71</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>7</v>
@@ -1219,33 +1542,799 @@
       <c r="A43" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B43" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C43" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="D43" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B44" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D43" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="37.799999999999997" customHeight="1">
-      <c r="A44" s="1"/>
-      <c r="B44" s="1"/>
-      <c r="C44" s="1"/>
-      <c r="D44" s="1"/>
+      <c r="C44" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="45" spans="1:4">
-      <c r="A45" s="1"/>
-      <c r="B45" s="1"/>
-      <c r="C45" s="1"/>
-      <c r="D45" s="1"/>
+      <c r="A45" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="46" spans="1:4">
-      <c r="A46" s="1"/>
-      <c r="B46" s="1"/>
-      <c r="C46" s="1"/>
-      <c r="D46" s="1"/>
+      <c r="A46" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="A66" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="A67" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="A68" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C69" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="A70" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C70" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
+      <c r="A71" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
+      <c r="A72" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
+      <c r="A73" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C73" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
+      <c r="A74" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
+      <c r="A75" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C75" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
+      <c r="A76" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
+      <c r="A77" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C77" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
+      <c r="A78" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C78" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
+      <c r="A79" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C79" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
+      <c r="A80" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C80" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4">
+      <c r="A81" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C81" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4">
+      <c r="A82" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C82" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
+      <c r="A83" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C83" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4">
+      <c r="A84" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C84" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4">
+      <c r="A85" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C85" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4">
+      <c r="A86" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C86" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4">
+      <c r="A87" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C87" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4">
+      <c r="A88" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C88" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4">
+      <c r="A89" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C89" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4">
+      <c r="A90" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C90" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4">
+      <c r="A91" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C91" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4">
+      <c r="A92" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="C92" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4">
+      <c r="A93" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C93" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4">
+      <c r="A94" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="C94" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4">
+      <c r="A95" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C95" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4">
+      <c r="A96" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C96" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4">
+      <c r="A97" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="C97" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4">
+      <c r="A98" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C98" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4">
+      <c r="A99" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="C99" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="1.5" right="1.5" top="1.5" bottom="1.5" header="0.5" footer="0.5"/>

</xml_diff>